<commit_message>
Lecture partielle de l'EDT M1 MIAGE.
</commit_message>
<xml_diff>
--- a/.xlsx
+++ b/.xlsx
@@ -12,119 +12,119 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2038" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2038" uniqueCount="159">
   <si>
     <t xml:space="preserve">Semaine : </t>
   </si>
   <si>
+    <t>lundi</t>
+  </si>
+  <si>
+    <t>Télécoms (KINX6AC1)</t>
+  </si>
+  <si>
+    <t>JGT</t>
+  </si>
+  <si>
+    <t>10:0</t>
+  </si>
+  <si>
+    <t>TYPE_AUTRE</t>
+  </si>
+  <si>
+    <t>PJ (KINR6AD2)</t>
+  </si>
+  <si>
+    <t>KINR6AD2</t>
+  </si>
+  <si>
+    <t>13:30</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>KINX6AC1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>JS</t>
+  </si>
+  <si>
+    <t>15:45</t>
+  </si>
+  <si>
+    <t>BE (KINR6AE1)</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>18:0</t>
+  </si>
+  <si>
+    <t>mardi</t>
+  </si>
+  <si>
+    <t>Anglais (KINR6AV1)</t>
+  </si>
+  <si>
+    <t>KINR6AV1</t>
+  </si>
+  <si>
+    <t>7:45</t>
+  </si>
+  <si>
+    <t>mercredi</t>
+  </si>
+  <si>
+    <t>CPO (KINX6AA1)</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>Réseaux d'opérateurs (KINX6AB1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tech. de  trans. /TPC (FM)  </t>
+  </si>
+  <si>
+    <t>FM</t>
+  </si>
+  <si>
     <t>jeudi</t>
   </si>
   <si>
-    <t>Télécoms (KINX6AC1)</t>
-  </si>
-  <si>
-    <t>JGT</t>
-  </si>
-  <si>
-    <t>10:0</t>
-  </si>
-  <si>
-    <t>TYPE_AUTRE</t>
-  </si>
-  <si>
-    <t>PJ (KINR6AD2)</t>
-  </si>
-  <si>
-    <t>KINR6AD2</t>
-  </si>
-  <si>
-    <t>13:30</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>KINX6AC1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>JS</t>
-  </si>
-  <si>
-    <t>15:45</t>
-  </si>
-  <si>
-    <t>BE (KINR6AE1)</t>
-  </si>
-  <si>
-    <t>AA</t>
-  </si>
-  <si>
-    <t>18:0</t>
+    <t>Réseaux (KINX5AC3) - CC</t>
+  </si>
+  <si>
+    <t>TG</t>
+  </si>
+  <si>
+    <t>TYPE_COURS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCP/IP (KINX6AB2) </t>
+  </si>
+  <si>
+    <t>Sport (KUPX6BA4)</t>
+  </si>
+  <si>
+    <t>KUPX6BA4</t>
+  </si>
+  <si>
+    <t>Informatique (KINR5AA1) (OM) / GC</t>
+  </si>
+  <si>
+    <t>KINR5AA1</t>
   </si>
   <si>
     <t>vendredi</t>
   </si>
   <si>
-    <t>Anglais (KINR6AV1)</t>
-  </si>
-  <si>
-    <t>KINR6AV1</t>
-  </si>
-  <si>
-    <t>7:45</t>
-  </si>
-  <si>
-    <t>samedi</t>
-  </si>
-  <si>
-    <t>CPO (KINX6AA1)</t>
-  </si>
-  <si>
-    <t>PT</t>
-  </si>
-  <si>
-    <t>Réseaux d'opérateurs (KINX6AB1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tech. de  trans. /TPC (FM)  </t>
-  </si>
-  <si>
-    <t>FM</t>
-  </si>
-  <si>
-    <t>dimanche</t>
-  </si>
-  <si>
-    <t>Réseaux (KINX5AC3) - CC</t>
-  </si>
-  <si>
-    <t>TG</t>
-  </si>
-  <si>
-    <t>TYPE_COURS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCP/IP (KINX6AB2) </t>
-  </si>
-  <si>
-    <t>Sport (KUPX6BA4)</t>
-  </si>
-  <si>
-    <t>KUPX6BA4</t>
-  </si>
-  <si>
-    <t>Informatique (KINR5AA1) (OM) / GC</t>
-  </si>
-  <si>
-    <t>KINR5AA1</t>
-  </si>
-  <si>
-    <t>lundi</t>
-  </si>
-  <si>
     <t>Anglais (KUPX6BA1)</t>
   </si>
   <si>
@@ -405,18 +405,6 @@
   </si>
   <si>
     <t>9:0</t>
-  </si>
-  <si>
-    <t>8:45</t>
-  </si>
-  <si>
-    <t>11:0</t>
-  </si>
-  <si>
-    <t>14:30</t>
-  </si>
-  <si>
-    <t>16:45</t>
   </si>
   <si>
     <t xml:space="preserve">Télécoms () (KINX6AC1) /TP/GC </t>
@@ -563,7 +551,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n" s="1">
-        <v>44931.0</v>
+        <v>46027.0</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>1</v>
@@ -680,7 +668,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n" s="1">
-        <v>44932.0</v>
+        <v>46028.0</v>
       </c>
       <c r="B8" t="s" s="0">
         <v>17</v>
@@ -753,7 +741,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n" s="1">
-        <v>44933.0</v>
+        <v>46029.0</v>
       </c>
       <c r="B12" t="s" s="0">
         <v>21</v>
@@ -870,7 +858,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n" s="1">
-        <v>44934.0</v>
+        <v>46030.0</v>
       </c>
       <c r="B18" t="s" s="0">
         <v>27</v>
@@ -987,7 +975,7 @@
     </row>
     <row r="24">
       <c r="A24" t="n" s="1">
-        <v>44935.0</v>
+        <v>46031.0</v>
       </c>
       <c r="B24" t="s" s="0">
         <v>36</v>
@@ -1095,7 +1083,7 @@
     </row>
     <row r="30">
       <c r="A30" t="n" s="1">
-        <v>44938.0</v>
+        <v>46034.0</v>
       </c>
       <c r="B30" t="s" s="0">
         <v>1</v>
@@ -1214,7 +1202,7 @@
     </row>
     <row r="36">
       <c r="A36" t="n" s="1">
-        <v>44939.0</v>
+        <v>46035.0</v>
       </c>
       <c r="B36" t="s" s="0">
         <v>17</v>
@@ -1306,7 +1294,7 @@
     </row>
     <row r="41">
       <c r="A41" t="n" s="1">
-        <v>44940.0</v>
+        <v>46036.0</v>
       </c>
       <c r="B41" t="s" s="0">
         <v>21</v>
@@ -1423,7 +1411,7 @@
     </row>
     <row r="47">
       <c r="A47" t="n" s="1">
-        <v>44941.0</v>
+        <v>46037.0</v>
       </c>
       <c r="B47" t="s" s="0">
         <v>27</v>
@@ -1590,7 +1578,7 @@
     </row>
     <row r="55">
       <c r="A55" t="n" s="1">
-        <v>44942.0</v>
+        <v>46038.0</v>
       </c>
       <c r="B55" t="s" s="0">
         <v>36</v>
@@ -1719,7 +1707,7 @@
     </row>
     <row r="62">
       <c r="A62" t="n" s="1">
-        <v>44945.0</v>
+        <v>46041.0</v>
       </c>
       <c r="B62" t="s" s="0">
         <v>1</v>
@@ -1911,7 +1899,7 @@
     </row>
     <row r="71">
       <c r="A71" t="n" s="1">
-        <v>44946.0</v>
+        <v>46042.0</v>
       </c>
       <c r="B71" t="s" s="0">
         <v>17</v>
@@ -1982,7 +1970,7 @@
     </row>
     <row r="75">
       <c r="A75" t="n" s="1">
-        <v>44947.0</v>
+        <v>46043.0</v>
       </c>
       <c r="B75" t="s" s="0">
         <v>21</v>
@@ -2078,7 +2066,7 @@
     </row>
     <row r="80">
       <c r="A80" t="n" s="1">
-        <v>44948.0</v>
+        <v>46044.0</v>
       </c>
       <c r="B80" t="s" s="0">
         <v>27</v>
@@ -2199,7 +2187,7 @@
     </row>
     <row r="86">
       <c r="A86" t="n" s="1">
-        <v>44949.0</v>
+        <v>46045.0</v>
       </c>
       <c r="B86" t="s" s="0">
         <v>36</v>
@@ -2326,7 +2314,7 @@
     </row>
     <row r="93">
       <c r="A93" t="n" s="1">
-        <v>44952.0</v>
+        <v>46048.0</v>
       </c>
       <c r="B93" t="s" s="0">
         <v>1</v>
@@ -2472,7 +2460,7 @@
     </row>
     <row r="100">
       <c r="A100" t="n" s="1">
-        <v>44953.0</v>
+        <v>46049.0</v>
       </c>
       <c r="B100" t="s" s="0">
         <v>17</v>
@@ -2639,7 +2627,7 @@
     </row>
     <row r="108">
       <c r="A108" t="n" s="1">
-        <v>44954.0</v>
+        <v>46050.0</v>
       </c>
       <c r="B108" t="s" s="0">
         <v>21</v>
@@ -2756,7 +2744,7 @@
     </row>
     <row r="114">
       <c r="A114" t="n" s="1">
-        <v>44955.0</v>
+        <v>46051.0</v>
       </c>
       <c r="B114" t="s" s="0">
         <v>27</v>
@@ -2971,7 +2959,7 @@
     </row>
     <row r="124">
       <c r="A124" t="n" s="1">
-        <v>44956.0</v>
+        <v>46052.0</v>
       </c>
       <c r="B124" t="s" s="0">
         <v>36</v>
@@ -3077,7 +3065,7 @@
     </row>
     <row r="130">
       <c r="A130" t="n" s="1">
-        <v>44959.0</v>
+        <v>46055.0</v>
       </c>
       <c r="B130" t="s" s="0">
         <v>1</v>
@@ -3223,7 +3211,7 @@
     </row>
     <row r="137">
       <c r="A137" t="n" s="1">
-        <v>44960.0</v>
+        <v>46056.0</v>
       </c>
       <c r="B137" t="s" s="0">
         <v>17</v>
@@ -3390,7 +3378,7 @@
     </row>
     <row r="145">
       <c r="A145" t="n" s="1">
-        <v>44961.0</v>
+        <v>46057.0</v>
       </c>
       <c r="B145" t="s" s="0">
         <v>21</v>
@@ -3532,7 +3520,7 @@
     </row>
     <row r="152">
       <c r="A152" t="n" s="1">
-        <v>44962.0</v>
+        <v>46058.0</v>
       </c>
       <c r="B152" t="s" s="0">
         <v>27</v>
@@ -3747,7 +3735,7 @@
     </row>
     <row r="162">
       <c r="A162" t="n" s="1">
-        <v>44963.0</v>
+        <v>46059.0</v>
       </c>
       <c r="B162" t="s" s="0">
         <v>36</v>
@@ -3830,7 +3818,7 @@
     </row>
     <row r="167">
       <c r="A167" t="n" s="1">
-        <v>44966.0</v>
+        <v>46062.0</v>
       </c>
       <c r="B167" t="s" s="0">
         <v>1</v>
@@ -3930,7 +3918,7 @@
     </row>
     <row r="172">
       <c r="A172" t="n" s="1">
-        <v>44967.0</v>
+        <v>46063.0</v>
       </c>
       <c r="B172" t="s" s="0">
         <v>17</v>
@@ -4030,7 +4018,7 @@
     </row>
     <row r="177">
       <c r="A177" t="n" s="1">
-        <v>44968.0</v>
+        <v>46064.0</v>
       </c>
       <c r="B177" t="s" s="0">
         <v>21</v>
@@ -4130,7 +4118,7 @@
     </row>
     <row r="182">
       <c r="A182" t="n" s="1">
-        <v>44969.0</v>
+        <v>46065.0</v>
       </c>
       <c r="B182" t="s" s="0">
         <v>27</v>
@@ -4230,7 +4218,7 @@
     </row>
     <row r="187">
       <c r="A187" t="n" s="1">
-        <v>44970.0</v>
+        <v>46066.0</v>
       </c>
       <c r="B187" t="s" s="0">
         <v>36</v>
@@ -4338,7 +4326,7 @@
     </row>
     <row r="193">
       <c r="A193" t="n" s="1">
-        <v>44973.0</v>
+        <v>46069.0</v>
       </c>
       <c r="B193" t="s" s="0">
         <v>1</v>
@@ -4438,7 +4426,7 @@
     </row>
     <row r="198">
       <c r="A198" t="n" s="1">
-        <v>44974.0</v>
+        <v>46070.0</v>
       </c>
       <c r="B198" t="s" s="0">
         <v>17</v>
@@ -4515,7 +4503,7 @@
     </row>
     <row r="202">
       <c r="A202" t="n" s="1">
-        <v>44975.0</v>
+        <v>46071.0</v>
       </c>
       <c r="B202" t="s" s="0">
         <v>21</v>
@@ -4615,7 +4603,7 @@
     </row>
     <row r="207">
       <c r="A207" t="n" s="1">
-        <v>44976.0</v>
+        <v>46072.0</v>
       </c>
       <c r="B207" t="s" s="0">
         <v>27</v>
@@ -4715,7 +4703,7 @@
     </row>
     <row r="212">
       <c r="A212" t="n" s="1">
-        <v>44977.0</v>
+        <v>46073.0</v>
       </c>
       <c r="B212" t="s" s="0">
         <v>36</v>
@@ -4823,7 +4811,7 @@
     </row>
     <row r="218">
       <c r="A218" t="n" s="1">
-        <v>44980.0</v>
+        <v>46076.0</v>
       </c>
       <c r="B218" t="s" s="0">
         <v>1</v>
@@ -4923,7 +4911,7 @@
     </row>
     <row r="223">
       <c r="A223" t="n" s="1">
-        <v>44981.0</v>
+        <v>46077.0</v>
       </c>
       <c r="B223" t="s" s="0">
         <v>17</v>
@@ -5023,7 +5011,7 @@
     </row>
     <row r="228">
       <c r="A228" t="n" s="1">
-        <v>44982.0</v>
+        <v>46078.0</v>
       </c>
       <c r="B228" t="s" s="0">
         <v>21</v>
@@ -5077,7 +5065,7 @@
     </row>
     <row r="231">
       <c r="A231" t="n" s="1">
-        <v>44983.0</v>
+        <v>46079.0</v>
       </c>
       <c r="B231" t="s" s="0">
         <v>27</v>
@@ -5177,7 +5165,7 @@
     </row>
     <row r="236">
       <c r="A236" t="n" s="1">
-        <v>44984.0</v>
+        <v>46080.0</v>
       </c>
       <c r="B236" t="s" s="0">
         <v>36</v>
@@ -5285,7 +5273,7 @@
     </row>
     <row r="242">
       <c r="A242" t="n" s="1">
-        <v>44994.0</v>
+        <v>46090.0</v>
       </c>
       <c r="B242" t="s" s="0">
         <v>1</v>
@@ -5381,7 +5369,7 @@
     </row>
     <row r="247">
       <c r="A247" t="n" s="1">
-        <v>44995.0</v>
+        <v>46091.0</v>
       </c>
       <c r="B247" t="s" s="0">
         <v>17</v>
@@ -5573,7 +5561,7 @@
     </row>
     <row r="256">
       <c r="A256" t="n" s="1">
-        <v>44996.0</v>
+        <v>46092.0</v>
       </c>
       <c r="B256" t="s" s="0">
         <v>21</v>
@@ -5738,7 +5726,7 @@
     </row>
     <row r="264">
       <c r="A264" t="n" s="1">
-        <v>44997.0</v>
+        <v>46093.0</v>
       </c>
       <c r="B264" t="s" s="0">
         <v>27</v>
@@ -5930,7 +5918,7 @@
     </row>
     <row r="273">
       <c r="A273" t="n" s="1">
-        <v>44998.0</v>
+        <v>46094.0</v>
       </c>
       <c r="B273" t="s" s="0">
         <v>36</v>
@@ -6084,7 +6072,7 @@
     </row>
     <row r="281">
       <c r="A281" t="n" s="1">
-        <v>45001.0</v>
+        <v>46097.0</v>
       </c>
       <c r="B281" t="s" s="0">
         <v>1</v>
@@ -6180,7 +6168,7 @@
     </row>
     <row r="286">
       <c r="A286" t="n" s="1">
-        <v>45002.0</v>
+        <v>46098.0</v>
       </c>
       <c r="B286" t="s" s="0">
         <v>17</v>
@@ -6372,7 +6360,7 @@
     </row>
     <row r="295">
       <c r="A295" t="n" s="1">
-        <v>45003.0</v>
+        <v>46099.0</v>
       </c>
       <c r="B295" t="s" s="0">
         <v>21</v>
@@ -6470,7 +6458,7 @@
     </row>
     <row r="300">
       <c r="A300" t="n" s="1">
-        <v>45004.0</v>
+        <v>46100.0</v>
       </c>
       <c r="B300" t="s" s="0">
         <v>27</v>
@@ -6637,7 +6625,7 @@
     </row>
     <row r="308">
       <c r="A308" t="n" s="1">
-        <v>45005.0</v>
+        <v>46101.0</v>
       </c>
       <c r="B308" t="s" s="0">
         <v>36</v>
@@ -6768,7 +6756,7 @@
     </row>
     <row r="315">
       <c r="A315" t="n" s="1">
-        <v>45008.0</v>
+        <v>46104.0</v>
       </c>
       <c r="B315" t="s" s="0">
         <v>1</v>
@@ -6889,7 +6877,7 @@
     </row>
     <row r="321">
       <c r="A321" t="n" s="1">
-        <v>45009.0</v>
+        <v>46105.0</v>
       </c>
       <c r="B321" t="s" s="0">
         <v>17</v>
@@ -7035,7 +7023,7 @@
     </row>
     <row r="328">
       <c r="A328" t="n" s="1">
-        <v>45010.0</v>
+        <v>46106.0</v>
       </c>
       <c r="B328" t="s" s="0">
         <v>21</v>
@@ -7112,7 +7100,7 @@
     </row>
     <row r="332">
       <c r="A332" t="n" s="1">
-        <v>45011.0</v>
+        <v>46107.0</v>
       </c>
       <c r="B332" t="s" s="0">
         <v>27</v>
@@ -7127,7 +7115,7 @@
         <v>72</v>
       </c>
       <c r="D333" t="s" s="0">
-        <v>131</v>
+        <v>20</v>
       </c>
       <c r="E333" t="n" s="0">
         <v>2.0</v>
@@ -7150,7 +7138,7 @@
         <v>49</v>
       </c>
       <c r="D334" t="s" s="0">
-        <v>132</v>
+        <v>4</v>
       </c>
       <c r="E334" t="n" s="0">
         <v>2.0</v>
@@ -7173,7 +7161,7 @@
         <v>33</v>
       </c>
       <c r="D335" t="s" s="0">
-        <v>133</v>
+        <v>8</v>
       </c>
       <c r="E335" t="n" s="0">
         <v>2.0</v>
@@ -7196,7 +7184,7 @@
         <v>74</v>
       </c>
       <c r="D336" t="s" s="0">
-        <v>133</v>
+        <v>8</v>
       </c>
       <c r="E336" t="n" s="0">
         <v>2.0</v>
@@ -7219,7 +7207,7 @@
         <v>118</v>
       </c>
       <c r="D337" t="s" s="0">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="E337" t="n" s="0">
         <v>2.0</v>
@@ -7242,7 +7230,7 @@
         <v>69</v>
       </c>
       <c r="D338" t="s" s="0">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="E338" t="n" s="0">
         <v>2.0</v>
@@ -7258,7 +7246,7 @@
     </row>
     <row r="339">
       <c r="A339" t="n" s="1">
-        <v>45012.0</v>
+        <v>46108.0</v>
       </c>
       <c r="B339" t="s" s="0">
         <v>36</v>
@@ -7335,7 +7323,7 @@
     </row>
     <row r="343">
       <c r="A343" t="s" s="0">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B343" s="0"/>
       <c r="C343" t="s" s="0">
@@ -7412,7 +7400,7 @@
     </row>
     <row r="347">
       <c r="A347" t="n" s="1">
-        <v>45015.0</v>
+        <v>46111.0</v>
       </c>
       <c r="B347" t="s" s="0">
         <v>1</v>
@@ -7420,7 +7408,7 @@
     </row>
     <row r="348">
       <c r="A348" t="s" s="0">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B348" s="0"/>
       <c r="C348" t="s" s="0">
@@ -7445,7 +7433,7 @@
       </c>
       <c r="B349" s="0"/>
       <c r="C349" t="s" s="0">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D349" t="s" s="0">
         <v>4</v>
@@ -7504,7 +7492,7 @@
     </row>
     <row r="352">
       <c r="A352" t="n" s="1">
-        <v>45016.0</v>
+        <v>46112.0</v>
       </c>
       <c r="B352" t="s" s="0">
         <v>17</v>
@@ -7512,7 +7500,7 @@
     </row>
     <row r="353">
       <c r="A353" t="s" s="0">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B353" s="0"/>
       <c r="C353" t="s" s="0">
@@ -7558,7 +7546,7 @@
     </row>
     <row r="355">
       <c r="A355" t="s" s="0">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B355" s="0"/>
       <c r="C355" t="s" s="0">
@@ -7650,7 +7638,7 @@
     </row>
     <row r="359">
       <c r="A359" t="n" s="1">
-        <v>45017.0</v>
+        <v>46113.0</v>
       </c>
       <c r="B359" t="s" s="0">
         <v>21</v>
@@ -7683,7 +7671,7 @@
       </c>
       <c r="B361" s="0"/>
       <c r="C361" t="s" s="0">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D361" t="s" s="0">
         <v>4</v>
@@ -7700,7 +7688,7 @@
     </row>
     <row r="362">
       <c r="A362" t="s" s="0">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B362" s="0"/>
       <c r="C362" t="s" s="0">
@@ -7769,11 +7757,11 @@
     </row>
     <row r="365">
       <c r="A365" t="s" s="0">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B365" s="0"/>
       <c r="C365" t="s" s="0">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D365" t="s" s="0">
         <v>16</v>
@@ -7792,7 +7780,7 @@
     </row>
     <row r="366">
       <c r="A366" t="n" s="1">
-        <v>45018.0</v>
+        <v>46114.0</v>
       </c>
       <c r="B366" t="s" s="0">
         <v>27</v>
@@ -7800,7 +7788,7 @@
     </row>
     <row r="367">
       <c r="A367" t="s" s="0">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B367" s="0"/>
       <c r="C367" t="s" s="0">
@@ -7823,7 +7811,7 @@
     </row>
     <row r="368">
       <c r="A368" t="s" s="0">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B368" s="0"/>
       <c r="C368" t="s" s="0">
@@ -7846,7 +7834,7 @@
     </row>
     <row r="369">
       <c r="A369" t="s" s="0">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B369" s="0"/>
       <c r="C369" t="s" s="0">
@@ -7938,7 +7926,7 @@
     </row>
     <row r="373">
       <c r="A373" t="s" s="0">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B373" s="0"/>
       <c r="C373" t="s" s="0">
@@ -7984,7 +7972,7 @@
     </row>
     <row r="375">
       <c r="A375" t="n" s="1">
-        <v>45019.0</v>
+        <v>46115.0</v>
       </c>
       <c r="B375" t="s" s="0">
         <v>36</v>
@@ -8061,7 +8049,7 @@
     </row>
     <row r="379">
       <c r="A379" t="s" s="0">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B379" s="0"/>
       <c r="C379" t="s" s="0">
@@ -8107,7 +8095,7 @@
     </row>
     <row r="381">
       <c r="A381" t="s" s="0">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B381" s="0"/>
       <c r="C381" t="s" s="0">
@@ -8161,7 +8149,7 @@
     </row>
     <row r="384">
       <c r="A384" t="n" s="1">
-        <v>45023.0</v>
+        <v>46119.0</v>
       </c>
       <c r="B384" t="s" s="0">
         <v>17</v>
@@ -8169,7 +8157,7 @@
     </row>
     <row r="385">
       <c r="A385" t="s" s="0">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B385" s="0"/>
       <c r="C385" t="s" s="0">
@@ -8192,7 +8180,7 @@
     </row>
     <row r="386">
       <c r="A386" t="s" s="0">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B386" s="0"/>
       <c r="C386" t="s" s="0">
@@ -8215,7 +8203,7 @@
     </row>
     <row r="387">
       <c r="A387" t="s" s="0">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B387" s="0"/>
       <c r="C387" t="s" s="0">
@@ -8238,11 +8226,11 @@
     </row>
     <row r="388">
       <c r="A388" t="s" s="0">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B388" s="0"/>
       <c r="C388" t="s" s="0">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D388" t="s" s="0">
         <v>13</v>
@@ -8261,7 +8249,7 @@
     </row>
     <row r="389">
       <c r="A389" t="n" s="1">
-        <v>45024.0</v>
+        <v>46120.0</v>
       </c>
       <c r="B389" t="s" s="0">
         <v>21</v>
@@ -8269,7 +8257,7 @@
     </row>
     <row r="390">
       <c r="A390" t="s" s="0">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B390" s="0"/>
       <c r="C390" t="s" s="0">
@@ -8292,7 +8280,7 @@
     </row>
     <row r="391">
       <c r="A391" t="s" s="0">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B391" s="0"/>
       <c r="C391" t="s" s="0">
@@ -8315,7 +8303,7 @@
     </row>
     <row r="392">
       <c r="A392" t="s" s="0">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B392" s="0"/>
       <c r="C392" t="s" s="0">
@@ -8338,7 +8326,7 @@
     </row>
     <row r="393">
       <c r="A393" t="s" s="0">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B393" s="0"/>
       <c r="C393" t="s" s="0">
@@ -8361,7 +8349,7 @@
     </row>
     <row r="394">
       <c r="A394" t="n" s="1">
-        <v>45025.0</v>
+        <v>46121.0</v>
       </c>
       <c r="B394" t="s" s="0">
         <v>27</v>
@@ -8392,7 +8380,7 @@
     </row>
     <row r="396">
       <c r="A396" t="s" s="0">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B396" s="0"/>
       <c r="C396" t="s" s="0">
@@ -8415,11 +8403,11 @@
     </row>
     <row r="397">
       <c r="A397" t="s" s="0">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B397" s="0"/>
       <c r="C397" t="s" s="0">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D397" t="s" s="0">
         <v>13</v>
@@ -8438,11 +8426,11 @@
     </row>
     <row r="398">
       <c r="A398" t="s" s="0">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B398" s="0"/>
       <c r="C398" t="s" s="0">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D398" t="s" s="0">
         <v>16</v>
@@ -8461,7 +8449,7 @@
     </row>
     <row r="399">
       <c r="A399" t="n" s="1">
-        <v>45026.0</v>
+        <v>46122.0</v>
       </c>
       <c r="B399" t="s" s="0">
         <v>36</v>
@@ -8469,7 +8457,7 @@
     </row>
     <row r="400">
       <c r="A400" t="s" s="0">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B400" s="0"/>
       <c r="C400" t="s" s="0">
@@ -8492,7 +8480,7 @@
     </row>
     <row r="401">
       <c r="A401" t="s" s="0">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B401" s="0"/>
       <c r="C401" t="s" s="0">
@@ -8523,7 +8511,7 @@
     </row>
     <row r="403">
       <c r="A403" t="n" s="1">
-        <v>45029.0</v>
+        <v>46125.0</v>
       </c>
       <c r="B403" t="s" s="0">
         <v>1</v>
@@ -8531,7 +8519,7 @@
     </row>
     <row r="404">
       <c r="A404" t="s" s="0">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B404" s="0"/>
       <c r="C404" t="s" s="0">
@@ -8554,7 +8542,7 @@
     </row>
     <row r="405">
       <c r="A405" t="s" s="0">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B405" s="0"/>
       <c r="C405" t="s" s="0">
@@ -8577,7 +8565,7 @@
     </row>
     <row r="406">
       <c r="A406" t="n" s="1">
-        <v>45030.0</v>
+        <v>46126.0</v>
       </c>
       <c r="B406" t="s" s="0">
         <v>17</v>
@@ -8585,11 +8573,11 @@
     </row>
     <row r="407">
       <c r="A407" t="s" s="0">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B407" s="0"/>
       <c r="C407" t="s" s="0">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D407" t="s" s="0">
         <v>8</v>
@@ -8631,7 +8619,7 @@
     </row>
     <row r="409">
       <c r="A409" t="n" s="1">
-        <v>45031.0</v>
+        <v>46127.0</v>
       </c>
       <c r="B409" t="s" s="0">
         <v>21</v>
@@ -8639,7 +8627,7 @@
     </row>
     <row r="410">
       <c r="A410" t="s" s="0">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B410" s="0"/>
       <c r="C410" t="s" s="0">
@@ -8662,11 +8650,11 @@
     </row>
     <row r="411">
       <c r="A411" t="s" s="0">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B411" s="0"/>
       <c r="C411" t="s" s="0">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D411" t="s" s="0">
         <v>4</v>
@@ -8685,7 +8673,7 @@
     </row>
     <row r="412">
       <c r="A412" t="s" s="0">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B412" s="0"/>
       <c r="C412" t="s" s="0">
@@ -8708,7 +8696,7 @@
     </row>
     <row r="413">
       <c r="A413" t="s" s="0">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B413" s="0"/>
       <c r="C413" t="s" s="0">
@@ -8731,7 +8719,7 @@
     </row>
     <row r="414">
       <c r="A414" t="n" s="1">
-        <v>45032.0</v>
+        <v>46128.0</v>
       </c>
       <c r="B414" t="s" s="0">
         <v>27</v>
@@ -8739,11 +8727,11 @@
     </row>
     <row r="415">
       <c r="A415" t="s" s="0">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B415" s="0"/>
       <c r="C415" t="s" s="0">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D415" t="s" s="0">
         <v>8</v>
@@ -8785,11 +8773,11 @@
     </row>
     <row r="417">
       <c r="A417" t="s" s="0">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B417" s="0"/>
       <c r="C417" t="s" s="0">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D417" t="s" s="0">
         <v>16</v>
@@ -8808,7 +8796,7 @@
     </row>
     <row r="418">
       <c r="A418" t="n" s="1">
-        <v>45033.0</v>
+        <v>46129.0</v>
       </c>
       <c r="B418" t="s" s="0">
         <v>36</v>
@@ -8816,7 +8804,7 @@
     </row>
     <row r="419">
       <c r="A419" t="s" s="0">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B419" s="0"/>
       <c r="C419" t="s" s="0">
@@ -8839,7 +8827,7 @@
     </row>
     <row r="420">
       <c r="A420" t="s" s="0">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B420" s="0"/>
       <c r="C420" t="s" s="0">
@@ -8870,7 +8858,7 @@
     </row>
     <row r="422">
       <c r="A422" t="n" s="1">
-        <v>45036.0</v>
+        <v>46132.0</v>
       </c>
       <c r="B422" t="s" s="0">
         <v>1</v>
@@ -8878,7 +8866,7 @@
     </row>
     <row r="423">
       <c r="A423" t="s" s="0">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B423" s="0"/>
       <c r="C423" t="s" s="0">
@@ -8901,11 +8889,11 @@
     </row>
     <row r="424">
       <c r="A424" t="s" s="0">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B424" s="0"/>
       <c r="C424" t="s" s="0">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D424" t="s" s="0">
         <v>13</v>
@@ -8924,7 +8912,7 @@
     </row>
     <row r="425">
       <c r="A425" t="n" s="1">
-        <v>45037.0</v>
+        <v>46133.0</v>
       </c>
       <c r="B425" t="s" s="0">
         <v>17</v>
@@ -8932,7 +8920,7 @@
     </row>
     <row r="426">
       <c r="A426" t="s" s="0">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B426" s="0"/>
       <c r="C426" t="s" s="0">
@@ -8978,7 +8966,7 @@
     </row>
     <row r="428">
       <c r="A428" t="s" s="0">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B428" s="0"/>
       <c r="C428" t="s" s="0">
@@ -9001,7 +8989,7 @@
     </row>
     <row r="429">
       <c r="A429" t="n" s="1">
-        <v>45038.0</v>
+        <v>46134.0</v>
       </c>
       <c r="B429" t="s" s="0">
         <v>21</v>
@@ -9009,11 +8997,11 @@
     </row>
     <row r="430">
       <c r="A430" t="s" s="0">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B430" s="0"/>
       <c r="C430" t="s" s="0">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D430" t="s" s="0">
         <v>8</v>
@@ -9032,7 +9020,7 @@
     </row>
     <row r="431">
       <c r="A431" t="s" s="0">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B431" s="0"/>
       <c r="C431" t="s" s="0">
@@ -9055,11 +9043,11 @@
     </row>
     <row r="432">
       <c r="A432" t="s" s="0">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B432" s="0"/>
       <c r="C432" t="s" s="0">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D432" t="s" s="0">
         <v>13</v>
@@ -9078,7 +9066,7 @@
     </row>
     <row r="433">
       <c r="A433" t="s" s="0">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B433" s="0"/>
       <c r="C433" t="s" s="0">
@@ -9101,7 +9089,7 @@
     </row>
     <row r="434">
       <c r="A434" t="s" s="0">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B434" s="0"/>
       <c r="C434" t="s" s="0">
@@ -9124,7 +9112,7 @@
     </row>
     <row r="435">
       <c r="A435" t="n" s="1">
-        <v>45039.0</v>
+        <v>46135.0</v>
       </c>
       <c r="B435" t="s" s="0">
         <v>27</v>
@@ -9132,11 +9120,11 @@
     </row>
     <row r="436">
       <c r="A436" t="s" s="0">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B436" s="0"/>
       <c r="C436" t="s" s="0">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D436" t="s" s="0">
         <v>8</v>
@@ -9155,7 +9143,7 @@
     </row>
     <row r="437">
       <c r="A437" t="s" s="0">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B437" s="0"/>
       <c r="C437" t="s" s="0">
@@ -9178,11 +9166,11 @@
     </row>
     <row r="438">
       <c r="A438" t="s" s="0">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B438" s="0"/>
       <c r="C438" t="s" s="0">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D438" t="s" s="0">
         <v>13</v>
@@ -9201,7 +9189,7 @@
     </row>
     <row r="439">
       <c r="A439" t="s" s="0">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B439" s="0"/>
       <c r="C439" t="s" s="0">
@@ -9224,7 +9212,7 @@
     </row>
     <row r="440">
       <c r="A440" t="n" s="1">
-        <v>45040.0</v>
+        <v>46136.0</v>
       </c>
       <c r="B440" t="s" s="0">
         <v>36</v>
@@ -9232,11 +9220,11 @@
     </row>
     <row r="441">
       <c r="A441" t="s" s="0">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B441" s="0"/>
       <c r="C441" t="s" s="0">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D441" t="s" s="0">
         <v>8</v>
@@ -9255,7 +9243,7 @@
     </row>
     <row r="442">
       <c r="A442" t="s" s="0">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B442" s="0"/>
       <c r="C442" t="s" s="0">
@@ -9278,11 +9266,11 @@
     </row>
     <row r="443">
       <c r="A443" t="s" s="0">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B443" s="0"/>
       <c r="C443" t="s" s="0">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D443" t="s" s="0">
         <v>13</v>
@@ -9301,7 +9289,7 @@
     </row>
     <row r="444">
       <c r="A444" t="s" s="0">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B444" s="0"/>
       <c r="C444" t="s" s="0">
@@ -9332,7 +9320,7 @@
     </row>
     <row r="446">
       <c r="A446" t="n" s="1">
-        <v>45050.0</v>
+        <v>46146.0</v>
       </c>
       <c r="B446" t="s" s="0">
         <v>1</v>
@@ -9340,7 +9328,7 @@
     </row>
     <row r="447">
       <c r="A447" t="s" s="0">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B447" s="0"/>
       <c r="C447" t="s" s="0">
@@ -9365,7 +9353,7 @@
       </c>
       <c r="B448" s="0"/>
       <c r="C448" t="s" s="0">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D448" t="s" s="0">
         <v>4</v>
@@ -9382,7 +9370,7 @@
     </row>
     <row r="449">
       <c r="A449" t="s" s="0">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B449" s="0"/>
       <c r="C449" t="s" s="0">
@@ -9405,7 +9393,7 @@
     </row>
     <row r="450">
       <c r="A450" t="s" s="0">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B450" s="0"/>
       <c r="C450" t="s" s="0">
@@ -9451,7 +9439,7 @@
     </row>
     <row r="452">
       <c r="A452" t="s" s="0">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B452" s="0"/>
       <c r="C452" t="s" s="0">
@@ -9474,7 +9462,7 @@
     </row>
     <row r="453">
       <c r="A453" t="n" s="1">
-        <v>45051.0</v>
+        <v>46147.0</v>
       </c>
       <c r="B453" t="s" s="0">
         <v>17</v>
@@ -9526,7 +9514,7 @@
     </row>
     <row r="456">
       <c r="A456" t="s" s="0">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B456" s="0"/>
       <c r="C456" t="s" s="0">
@@ -9572,7 +9560,7 @@
     </row>
     <row r="458">
       <c r="A458" t="n" s="1">
-        <v>45052.0</v>
+        <v>46148.0</v>
       </c>
       <c r="B458" t="s" s="0">
         <v>21</v>
@@ -9626,7 +9614,7 @@
     </row>
     <row r="461">
       <c r="A461" t="s" s="0">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B461" s="0"/>
       <c r="C461" t="s" s="0">
@@ -9649,7 +9637,7 @@
     </row>
     <row r="462">
       <c r="A462" t="s" s="0">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B462" s="0"/>
       <c r="C462" t="s" s="0">
@@ -9695,7 +9683,7 @@
     </row>
     <row r="464">
       <c r="A464" t="s" s="0">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B464" s="0"/>
       <c r="C464" t="s" s="0">
@@ -9718,7 +9706,7 @@
     </row>
     <row r="465">
       <c r="A465" t="n" s="1">
-        <v>45053.0</v>
+        <v>46149.0</v>
       </c>
       <c r="B465" t="s" s="0">
         <v>27</v>
@@ -9726,7 +9714,7 @@
     </row>
     <row r="466">
       <c r="A466" t="s" s="0">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B466" s="0"/>
       <c r="C466" t="s" s="0">
@@ -9751,7 +9739,7 @@
       </c>
       <c r="B467" s="0"/>
       <c r="C467" t="s" s="0">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D467" t="s" s="0">
         <v>4</v>
@@ -9791,7 +9779,7 @@
     </row>
     <row r="469">
       <c r="A469" t="s" s="0">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B469" s="0"/>
       <c r="C469" t="s" s="0">
@@ -9814,11 +9802,11 @@
     </row>
     <row r="470">
       <c r="A470" t="s" s="0">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B470" s="0"/>
       <c r="C470" t="s" s="0">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D470" t="s" s="0">
         <v>13</v>
@@ -9837,7 +9825,7 @@
     </row>
     <row r="471">
       <c r="A471" t="s" s="0">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B471" s="0"/>
       <c r="C471" t="s" s="0">
@@ -9891,7 +9879,7 @@
     </row>
     <row r="474">
       <c r="A474" t="n" s="1">
-        <v>45057.0</v>
+        <v>46153.0</v>
       </c>
       <c r="B474" t="s" s="0">
         <v>1</v>
@@ -9926,7 +9914,7 @@
       </c>
       <c r="B476" s="0"/>
       <c r="C476" t="s" s="0">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D476" t="s" s="0">
         <v>4</v>
@@ -9964,7 +9952,7 @@
     </row>
     <row r="478">
       <c r="A478" t="s" s="0">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B478" s="0"/>
       <c r="C478" t="s" s="0">
@@ -9987,7 +9975,7 @@
     </row>
     <row r="479">
       <c r="A479" t="s" s="0">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B479" s="0"/>
       <c r="C479" t="s" s="0">
@@ -10010,7 +9998,7 @@
     </row>
     <row r="480">
       <c r="A480" t="s" s="0">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B480" s="0"/>
       <c r="C480" t="s" s="0">
@@ -10033,7 +10021,7 @@
     </row>
     <row r="481">
       <c r="A481" t="s" s="0">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B481" s="0"/>
       <c r="C481" t="s" s="0">
@@ -10056,7 +10044,7 @@
     </row>
     <row r="482">
       <c r="A482" t="n" s="1">
-        <v>45058.0</v>
+        <v>46154.0</v>
       </c>
       <c r="B482" t="s" s="0">
         <v>17</v>
@@ -10064,7 +10052,7 @@
     </row>
     <row r="483">
       <c r="A483" t="s" s="0">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B483" s="0"/>
       <c r="C483" t="s" s="0">
@@ -10110,7 +10098,7 @@
     </row>
     <row r="485">
       <c r="A485" t="s" s="0">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B485" s="0"/>
       <c r="C485" t="s" s="0">
@@ -10156,7 +10144,7 @@
     </row>
     <row r="487">
       <c r="A487" t="s" s="0">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B487" s="0"/>
       <c r="C487" t="s" s="0">
@@ -10200,7 +10188,7 @@
     </row>
     <row r="489">
       <c r="A489" t="n" s="1">
-        <v>45059.0</v>
+        <v>46155.0</v>
       </c>
       <c r="B489" t="s" s="0">
         <v>21</v>
@@ -10262,7 +10250,7 @@
     </row>
     <row r="493">
       <c r="A493" t="n" s="1">
-        <v>45064.0</v>
+        <v>46160.0</v>
       </c>
       <c r="B493" t="s" s="0">
         <v>1</v>
@@ -10270,11 +10258,11 @@
     </row>
     <row r="494">
       <c r="A494" t="s" s="0">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B494" s="0"/>
       <c r="C494" t="s" s="0">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D494" t="s" s="0">
         <v>20</v>
@@ -10293,7 +10281,7 @@
     </row>
     <row r="495">
       <c r="A495" t="s" s="0">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B495" s="0"/>
       <c r="C495" t="s" s="0">
@@ -10316,11 +10304,11 @@
     </row>
     <row r="496">
       <c r="A496" t="s" s="0">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B496" s="0"/>
       <c r="C496" t="s" s="0">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D496" t="s" s="0">
         <v>4</v>
@@ -10339,7 +10327,7 @@
     </row>
     <row r="497">
       <c r="A497" t="s" s="0">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B497" s="0"/>
       <c r="C497" t="s" s="0">
@@ -10362,7 +10350,7 @@
     </row>
     <row r="498">
       <c r="A498" t="n" s="1">
-        <v>45065.0</v>
+        <v>46161.0</v>
       </c>
       <c r="B498" t="s" s="0">
         <v>17</v>
@@ -10393,11 +10381,11 @@
     </row>
     <row r="500">
       <c r="A500" t="s" s="0">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B500" s="0"/>
       <c r="C500" t="s" s="0">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D500" t="s" s="0">
         <v>4</v>
@@ -10414,7 +10402,7 @@
     </row>
     <row r="501">
       <c r="A501" t="n" s="1">
-        <v>45066.0</v>
+        <v>46162.0</v>
       </c>
       <c r="B501" t="s" s="0">
         <v>21</v>
@@ -10422,11 +10410,11 @@
     </row>
     <row r="502">
       <c r="A502" t="s" s="0">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B502" s="0"/>
       <c r="C502" t="s" s="0">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D502" t="s" s="0">
         <v>4</v>

</xml_diff>